<commit_message>
Updated and corrected the analysis of cross section and fracture young modulus
</commit_message>
<xml_diff>
--- a/Results_and_analysis/Dependence_tensor_on_cross_section/results_analysis_complete_cross_section.xlsx
+++ b/Results_and_analysis/Dependence_tensor_on_cross_section/results_analysis_complete_cross_section.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plocha\Bachelor_thesis\Results_and_analysis\Dependence_tensor_on_cross_section\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60DD835-8FF3-4C8E-955B-CD89E7DBAA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA0D34C-6035-4B01-A477-5CEDE296089C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{434BF738-8343-4BA8-9715-0445CC697F35}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>C1</t>
   </si>
@@ -72,10 +72,13 @@
     <t>σ/μ [%]</t>
   </si>
   <si>
-    <t>COEFFICIENTS OF EFFECTIVE ELASTIC TENSOR</t>
+    <t>cross section multiplier value</t>
   </si>
   <si>
-    <t>cross section multiplier value</t>
+    <t>COEFFICIENTS OF EFFECTIVE ELASTIC TENSOR - TENSION</t>
+  </si>
+  <si>
+    <t>COEFFICIENTS OF EFFECTIVE ELASTIC TENSOR - COMPRESSION</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="cs-CZ" baseline="0"/>
-              <a:t> hodnot efektivních elastických koeficientů na cross section (multiplier = value, protože region je 1x1)</a:t>
+              <a:t> hodnot efektivních elastických koeficientů na cross section (oblast 1x1), tah 7%</a:t>
             </a:r>
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
@@ -522,7 +525,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.2373072553654869E-2"/>
+          <c:y val="7.6414454932402898E-2"/>
+          <c:w val="0.86938377377405274"/>
+          <c:h val="0.8119099306687293"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -558,10 +571,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -569,61 +582,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$C$4:$C$12</c:f>
+              <c:f>List1!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3338.0180527141101</c:v>
+                  <c:v>2348434433.5337701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2975.3897192631598</c:v>
+                  <c:v>1985055457.4479699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2461.7253697994101</c:v>
+                  <c:v>1852427823.27141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2441.7245797958599</c:v>
+                  <c:v>1781637161.21468</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3837.21792541782</c:v>
+                  <c:v>1736618346.0926399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1651.16549676006</c:v>
+                  <c:v>1705038862.71381</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1774.9440727178701</c:v>
+                  <c:v>1681368472.5090001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2312.8243541470802</c:v>
+                  <c:v>1662690100.2637801</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2450.7967912035901</c:v>
+                  <c:v>1647430283.5880899</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1634629202.83779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -667,10 +686,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -678,61 +697,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$D$4:$D$12</c:f>
+              <c:f>List1!$D$4:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-263.804307828726</c:v>
+                  <c:v>100451065.527909</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79.276510744169101</c:v>
+                  <c:v>70821950.867204696</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.5301755547144</c:v>
+                  <c:v>59564568.213844299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.2898157053168</c:v>
+                  <c:v>53969184.625737898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>207.80580231433899</c:v>
+                  <c:v>50656621.985981204</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.747819730912999</c:v>
+                  <c:v>48207462.722703502</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5111155206910096</c:v>
+                  <c:v>46201340.577220403</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.106867917505301</c:v>
+                  <c:v>44631028.642312303</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>152.31623757459599</c:v>
+                  <c:v>43353041.206873402</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42283229.505063698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -776,10 +801,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -787,61 +812,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$E$4:$E$12</c:f>
+              <c:f>List1!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>44.685357237618803</c:v>
+                  <c:v>19845860.245272499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-106.87964013101799</c:v>
+                  <c:v>-17796521.9256359</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.899761953312501</c:v>
+                  <c:v>-31849198.054356199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.0650904447436993</c:v>
+                  <c:v>-39630076.294682197</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>221.231677677785</c:v>
+                  <c:v>-44775736.351110399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.472437942975901</c:v>
+                  <c:v>-48550179.099549703</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.113392909110303</c:v>
+                  <c:v>-51484075.388887502</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-110.586619880323</c:v>
+                  <c:v>-53870825.145849697</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>66.649852041400393</c:v>
+                  <c:v>-55875547.492941201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-57599044.825210698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,10 +916,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -896,61 +927,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$F$4:$F$12</c:f>
+              <c:f>List1!$F$4:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>107.197720064202</c:v>
+                  <c:v>102933897.496317</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.947297553105599</c:v>
+                  <c:v>71443231.415179506</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.831851044362999</c:v>
+                  <c:v>59666946.698082097</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.382910900777102</c:v>
+                  <c:v>53284885.443142898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210.04935590016399</c:v>
+                  <c:v>49288956.961299904</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.1671353251332</c:v>
+                  <c:v>46527263.374106199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9157215855259704</c:v>
+                  <c:v>44471587.385885097</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.532608087494101</c:v>
+                  <c:v>42858109.674520902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>150.052604795143</c:v>
+                  <c:v>41542787.465746596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40440854.412757099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,10 +1031,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -1005,61 +1042,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$G$4:$G$12</c:f>
+              <c:f>List1!$G$4:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3239.8068802715402</c:v>
+                  <c:v>2425339833.0624099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2861.2205868238202</c:v>
+                  <c:v>2043896598.05389</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2112.9014778281598</c:v>
+                  <c:v>1904063940.8522201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2543.4392873532202</c:v>
+                  <c:v>1828700037.06126</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3734.22542610454</c:v>
+                  <c:v>1780116252.25035</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2358.5053043222001</c:v>
+                  <c:v>1745409527.05949</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2006.0377739957501</c:v>
+                  <c:v>1718952854.7392199</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2278.1066615201098</c:v>
+                  <c:v>1697874710.61129</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2462.97302699281</c:v>
+                  <c:v>1680541205.4347301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1665944400.1963601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1103,10 +1146,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -1114,61 +1157,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$H$4:$H$12</c:f>
+              <c:f>List1!$H$4:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>151.88636552243199</c:v>
+                  <c:v>33809222.398981698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-100.023409021246</c:v>
+                  <c:v>-3324531.1763485</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-52.7958041033977</c:v>
+                  <c:v>-17689999.295574401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-71.354243033971997</c:v>
+                  <c:v>-25508569.3399878</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>421.54242079011499</c:v>
+                  <c:v>-30709209.112047099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.87018324131401</c:v>
+                  <c:v>-34585162.749898203</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.754518218258703</c:v>
+                  <c:v>-37671032.541643202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-102.794114369748</c:v>
+                  <c:v>-40229262.9549798</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.85032153708717095</c:v>
+                  <c:v>-42405800.102588303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-44290987.609665699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1218,10 +1267,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -1229,61 +1278,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$I$4:$I$12</c:f>
+              <c:f>List1!$I$4:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>95.608423822010707</c:v>
+                  <c:v>19585310.3809288</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-114.89168764895599</c:v>
+                  <c:v>-15996358.8687004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.010313696825101</c:v>
+                  <c:v>-29983955.871647801</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-9.6671530760184101</c:v>
+                  <c:v>-37516436.928591803</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>220.69408854762801</c:v>
+                  <c:v>-42388453.401578203</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.742876947719601</c:v>
+                  <c:v>-45928619.199056603</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.272528087686794</c:v>
+                  <c:v>-48702880.547294699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-108.501817073186</c:v>
+                  <c:v>-50986752.507453904</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>68.777145392852006</c:v>
+                  <c:v>-52929554.844482496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-54619959.289673798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,10 +1388,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -1344,61 +1399,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$J$4:$J$12</c:f>
+              <c:f>List1!$J$4:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35.3754284797011</c:v>
+                  <c:v>18533668.903669499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-104.328880834095</c:v>
+                  <c:v>-538615.47619490698</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-54.181999534598901</c:v>
+                  <c:v>-14735444.4272255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-73.814088301716495</c:v>
+                  <c:v>-22648176.148858499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>420.42892621605802</c:v>
+                  <c:v>-27911794.4661965</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>131.01183412173299</c:v>
+                  <c:v>-31791034.411033001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37.703050505763301</c:v>
+                  <c:v>-34832577.169397101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-106.3424810918</c:v>
+                  <c:v>-37311702.137431502</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6199618616344999E-2</c:v>
+                  <c:v>-39385145.744099602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-41151499.8668897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,10 +1509,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$B$4:$B$12</c:f>
+              <c:f>List1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
                 </c:pt>
@@ -1459,61 +1520,67 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.84</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$K$4:$K$12</c:f>
+              <c:f>List1!$K$4:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1124.6535185696</c:v>
+                  <c:v>713243397.28215098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>599.751545769122</c:v>
+                  <c:v>512068013.39598799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>370.43267096227902</c:v>
+                  <c:v>442579153.78078401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>485.13108096400998</c:v>
+                  <c:v>405438349.42229903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1050.40903293614</c:v>
+                  <c:v>381733886.893727</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>209.49603349467299</c:v>
+                  <c:v>364921524.65888798</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240.549107507809</c:v>
+                  <c:v>352140630.55937803</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>351.689425069381</c:v>
+                  <c:v>341944057.71948701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>680.35616504010295</c:v>
+                  <c:v>333520386.40840602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>326377888.19770199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1540,7 +1607,7 @@
         <c:axId val="1131194959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1559,6 +1626,44 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Kolikrát je menší</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="cs-CZ" baseline="0"/>
+                  <a:t> cross section vůči velikosti oblasti</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42696273492239351"/>
+              <c:y val="0.91716780347801652"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1633,7 +1738,8 @@
         <c:axId val="1131193999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4000"/>
+          <c:max val="2425339833"/>
+          <c:min val="-300000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1652,6 +1758,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Hodnota efektivních konstant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1805,7 +1936,1536 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Graf závislosti hodnot efektivních elastických koeficientů na cross section (oblast 1x1), komprese 7%</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8660485765504815E-2"/>
+          <c:y val="8.6357659065109643E-2"/>
+          <c:w val="0.84673352869344087"/>
+          <c:h val="0.84422879936067396"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>C1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$R$4:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2354465672.4657001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1984837287.03004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1852215801.2544899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1781497863.3529</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1736557325.7691801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1705038862.71381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1681368472.5090001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1662690100.2637801</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1647430283.5880899</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1634629202.83779</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>C2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$S$4:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>105740501.36530399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72488992.228721395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60594575.650751904</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54516327.467568897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50833911.157726496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48207462.722703502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46201340.577220403</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44631028.642312303</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43353041.206873402</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42283229.505063698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>C3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$T$4:$T$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>18247660.305660401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-18465232.9993321</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-32208001.899628699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-39806112.892950602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-44817910.385637604</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-48550179.099549703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-51484075.388887502</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-53870825.145849697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-55875547.492941201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-57599044.825210698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>C4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$U$4:$U$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>101795217.65406799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71454520.490679905</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59708813.230726004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53284885.443142898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49288956.961299904</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46527263.374106199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44471587.385885097</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42858109.674520902</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41542787.465746596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40440854.412757099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>C5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$V$4:$V$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2471800046.8102102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2044259773.5499499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1904032155.1886001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1828700037.06126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1780116252.25035</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1745409527.05949</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1718952854.7392199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1697874710.61129</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1680541205.4347301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1665944400.1963601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>C6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$W$4:$W$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>29824250.833563101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3535934.06757739</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-17721431.171448398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-25508569.3399878</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-30709209.112047099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-34585162.749898203</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-37671032.541643202</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-40229262.9549798</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-42405800.102588303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-44290987.609665699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>C7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$X$4:$X$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30041091.732397102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-15996358.8687004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-29983955.871647801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-37516436.928591803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-42388453.401578203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-45928619.199056603</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-48702880.547294699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-50986752.507453904</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-52929554.844482496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-54619959.289673798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>C8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$Y$4:$Y$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57214258.017845802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-538615.47619490698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14735444.4272255</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-22648176.148858499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-27911794.4661965</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-31791034.411033001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-34832577.169397101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-37311702.137431502</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-39385145.744099602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-41151499.8668897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>C9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$Z$4:$Z$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>716861889.58415699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512068013.39598799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>442579153.78078401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>405438349.42229903</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>381733886.893727</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>364921524.65888798</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>352140630.55937803</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>341944057.71948701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>333520386.40840602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>326377888.19770199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-E4A2-443D-9049-5AD9BB6A9BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1621004752"/>
+        <c:axId val="1621006672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1621004752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Kolikrát je menší cross section vůči velikosti oblasti</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1621006672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1621006672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2500000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Hodnota efektivních konstant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1621004752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2361,20 +4021,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>288924</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:colOff>584528</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>98096</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>86994</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>175173</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>120432</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2394,6 +4570,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>21165</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>162983</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>1045881</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graf 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E835BEE1-E304-B032-82FB-206B65D7F839}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2699,28 +4911,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47630F0-D406-4D99-ACD0-4230A5574627}">
-  <dimension ref="B1:K15"/>
+  <dimension ref="B1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -2730,8 +4941,22 @@
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
+      <c r="Q2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
     </row>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="18"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -2760,424 +4985,923 @@
       <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>0.01</v>
       </c>
       <c r="C4" s="4">
-        <v>3338.0180527141101</v>
+        <v>2348434433.5337701</v>
       </c>
       <c r="D4" s="5">
-        <v>-263.804307828726</v>
+        <v>100451065.527909</v>
       </c>
       <c r="E4" s="5">
-        <v>44.685357237618803</v>
+        <v>19845860.245272499</v>
       </c>
       <c r="F4" s="5">
-        <v>107.197720064202</v>
+        <v>102933897.496317</v>
       </c>
       <c r="G4" s="5">
-        <v>3239.8068802715402</v>
+        <v>2425339833.0624099</v>
       </c>
       <c r="H4" s="5">
-        <v>151.88636552243199</v>
+        <v>33809222.398981698</v>
       </c>
       <c r="I4" s="5">
-        <v>95.608423822010707</v>
+        <v>19585310.3809288</v>
       </c>
       <c r="J4" s="5">
-        <v>35.3754284797011</v>
+        <v>18533668.903669499</v>
       </c>
       <c r="K4" s="5">
-        <v>1124.6535185696</v>
+        <v>713243397.28215098</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="R4" s="4">
+        <v>2354465672.4657001</v>
+      </c>
+      <c r="S4" s="5">
+        <v>105740501.36530399</v>
+      </c>
+      <c r="T4" s="5">
+        <v>18247660.305660401</v>
+      </c>
+      <c r="U4" s="5">
+        <v>101795217.65406799</v>
+      </c>
+      <c r="V4" s="5">
+        <v>2471800046.8102102</v>
+      </c>
+      <c r="W4" s="5">
+        <v>29824250.833563101</v>
+      </c>
+      <c r="X4" s="5">
+        <v>30041091.732397102</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>57214258.017845802</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>716861889.58415699</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B5" s="6">
         <v>0.02</v>
       </c>
       <c r="C5">
-        <v>2975.3897192631598</v>
+        <v>1985055457.4479699</v>
       </c>
       <c r="D5" s="7">
-        <v>79.276510744169101</v>
+        <v>70821950.867204696</v>
       </c>
       <c r="E5" s="7">
-        <v>-106.87964013101799</v>
+        <v>-17796521.9256359</v>
       </c>
       <c r="F5" s="7">
-        <v>78.947297553105599</v>
+        <v>71443231.415179506</v>
       </c>
       <c r="G5" s="7">
-        <v>2861.2205868238202</v>
+        <v>2043896598.05389</v>
       </c>
       <c r="H5" s="7">
-        <v>-100.023409021246</v>
+        <v>-3324531.1763485</v>
       </c>
       <c r="I5" s="7">
-        <v>-114.89168764895599</v>
+        <v>-15996358.8687004</v>
       </c>
       <c r="J5" s="7">
-        <v>-104.328880834095</v>
+        <v>-538615.47619490698</v>
       </c>
       <c r="K5" s="7">
-        <v>599.751545769122</v>
+        <v>512068013.39598799</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="R5">
+        <v>1984837287.03004</v>
+      </c>
+      <c r="S5" s="7">
+        <v>72488992.228721395</v>
+      </c>
+      <c r="T5" s="7">
+        <v>-18465232.9993321</v>
+      </c>
+      <c r="U5" s="7">
+        <v>71454520.490679905</v>
+      </c>
+      <c r="V5" s="7">
+        <v>2044259773.5499499</v>
+      </c>
+      <c r="W5" s="7">
+        <v>-3535934.06757739</v>
+      </c>
+      <c r="X5" s="7">
+        <v>-15996358.8687004</v>
+      </c>
+      <c r="Y5" s="7">
+        <v>-538615.47619490698</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>512068013.39598799</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="C6">
+        <v>1852427823.27141</v>
+      </c>
+      <c r="D6" s="7">
+        <v>59564568.213844299</v>
+      </c>
+      <c r="E6" s="7">
+        <v>-31849198.054356199</v>
+      </c>
+      <c r="F6" s="7">
+        <v>59666946.698082097</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1904063940.8522201</v>
+      </c>
+      <c r="H6" s="7">
+        <v>-17689999.295574401</v>
+      </c>
+      <c r="I6" s="7">
+        <v>-29983955.871647801</v>
+      </c>
+      <c r="J6" s="7">
+        <v>-14735444.4272255</v>
+      </c>
+      <c r="K6" s="7">
+        <v>442579153.78078401</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="R6">
+        <v>1852215801.2544899</v>
+      </c>
+      <c r="S6" s="7">
+        <v>60594575.650751904</v>
+      </c>
+      <c r="T6" s="7">
+        <v>-32208001.899628699</v>
+      </c>
+      <c r="U6" s="7">
+        <v>59708813.230726004</v>
+      </c>
+      <c r="V6" s="7">
+        <v>1904032155.1886001</v>
+      </c>
+      <c r="W6" s="7">
+        <v>-17721431.171448398</v>
+      </c>
+      <c r="X6" s="7">
+        <v>-29983955.871647801</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>-14735444.4272255</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>442579153.78078401</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B7" s="6">
         <v>0.04</v>
       </c>
-      <c r="C6">
-        <v>2461.7253697994101</v>
-      </c>
-      <c r="D6" s="7">
-        <v>28.5301755547144</v>
-      </c>
-      <c r="E6" s="7">
-        <v>15.899761953312501</v>
-      </c>
-      <c r="F6" s="7">
-        <v>28.831851044362999</v>
-      </c>
-      <c r="G6" s="7">
-        <v>2112.9014778281598</v>
-      </c>
-      <c r="H6" s="7">
-        <v>-52.7958041033977</v>
-      </c>
-      <c r="I6" s="7">
-        <v>19.010313696825101</v>
-      </c>
-      <c r="J6" s="7">
-        <v>-54.181999534598901</v>
-      </c>
-      <c r="K6" s="7">
-        <v>370.43267096227902</v>
+      <c r="C7">
+        <v>1781637161.21468</v>
+      </c>
+      <c r="D7" s="7">
+        <v>53969184.625737898</v>
+      </c>
+      <c r="E7" s="7">
+        <v>-39630076.294682197</v>
+      </c>
+      <c r="F7" s="7">
+        <v>53284885.443142898</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1828700037.06126</v>
+      </c>
+      <c r="H7" s="7">
+        <v>-25508569.3399878</v>
+      </c>
+      <c r="I7" s="7">
+        <v>-37516436.928591803</v>
+      </c>
+      <c r="J7" s="7">
+        <v>-22648176.148858499</v>
+      </c>
+      <c r="K7" s="7">
+        <v>405438349.42229903</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="R7">
+        <v>1781497863.3529</v>
+      </c>
+      <c r="S7" s="7">
+        <v>54516327.467568897</v>
+      </c>
+      <c r="T7" s="7">
+        <v>-39806112.892950602</v>
+      </c>
+      <c r="U7" s="7">
+        <v>53284885.443142898</v>
+      </c>
+      <c r="V7" s="7">
+        <v>1828700037.06126</v>
+      </c>
+      <c r="W7" s="7">
+        <v>-25508569.3399878</v>
+      </c>
+      <c r="X7" s="7">
+        <v>-37516436.928591803</v>
+      </c>
+      <c r="Y7" s="7">
+        <v>-22648176.148858499</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>405438349.42229903</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="6">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C8">
+        <v>1736618346.0926399</v>
+      </c>
+      <c r="D8" s="7">
+        <v>50656621.985981204</v>
+      </c>
+      <c r="E8" s="7">
+        <v>-44775736.351110399</v>
+      </c>
+      <c r="F8" s="7">
+        <v>49288956.961299904</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1780116252.25035</v>
+      </c>
+      <c r="H8" s="7">
+        <v>-30709209.112047099</v>
+      </c>
+      <c r="I8" s="7">
+        <v>-42388453.401578203</v>
+      </c>
+      <c r="J8" s="7">
+        <v>-27911794.4661965</v>
+      </c>
+      <c r="K8" s="7">
+        <v>381733886.893727</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="R8">
+        <v>1736557325.7691801</v>
+      </c>
+      <c r="S8" s="7">
+        <v>50833911.157726496</v>
+      </c>
+      <c r="T8" s="7">
+        <v>-44817910.385637604</v>
+      </c>
+      <c r="U8" s="7">
+        <v>49288956.961299904</v>
+      </c>
+      <c r="V8" s="7">
+        <v>1780116252.25035</v>
+      </c>
+      <c r="W8" s="7">
+        <v>-30709209.112047099</v>
+      </c>
+      <c r="X8" s="7">
+        <v>-42388453.401578203</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>-27911794.4661965</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>381733886.893727</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B9" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="C9">
+        <v>1705038862.71381</v>
+      </c>
+      <c r="D9" s="7">
+        <v>48207462.722703502</v>
+      </c>
+      <c r="E9" s="7">
+        <v>-48550179.099549703</v>
+      </c>
+      <c r="F9" s="7">
+        <v>46527263.374106199</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1745409527.05949</v>
+      </c>
+      <c r="H9" s="7">
+        <v>-34585162.749898203</v>
+      </c>
+      <c r="I9" s="7">
+        <v>-45928619.199056603</v>
+      </c>
+      <c r="J9" s="7">
+        <v>-31791034.411033001</v>
+      </c>
+      <c r="K9" s="7">
+        <v>364921524.65888798</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="R9">
+        <v>1705038862.71381</v>
+      </c>
+      <c r="S9" s="7">
+        <v>48207462.722703502</v>
+      </c>
+      <c r="T9" s="7">
+        <v>-48550179.099549703</v>
+      </c>
+      <c r="U9" s="7">
+        <v>46527263.374106199</v>
+      </c>
+      <c r="V9" s="7">
+        <v>1745409527.05949</v>
+      </c>
+      <c r="W9" s="7">
+        <v>-34585162.749898203</v>
+      </c>
+      <c r="X9" s="7">
+        <v>-45928619.199056603</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>-31791034.411033001</v>
+      </c>
+      <c r="Z9" s="7">
+        <v>364921524.65888798</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C10">
+        <v>1681368472.5090001</v>
+      </c>
+      <c r="D10" s="7">
+        <v>46201340.577220403</v>
+      </c>
+      <c r="E10" s="7">
+        <v>-51484075.388887502</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44471587.385885097</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1718952854.7392199</v>
+      </c>
+      <c r="H10" s="7">
+        <v>-37671032.541643202</v>
+      </c>
+      <c r="I10" s="7">
+        <v>-48702880.547294699</v>
+      </c>
+      <c r="J10" s="7">
+        <v>-34832577.169397101</v>
+      </c>
+      <c r="K10" s="7">
+        <v>352140630.55937803</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R10">
+        <v>1681368472.5090001</v>
+      </c>
+      <c r="S10" s="7">
+        <v>46201340.577220403</v>
+      </c>
+      <c r="T10" s="7">
+        <v>-51484075.388887502</v>
+      </c>
+      <c r="U10" s="7">
+        <v>44471587.385885097</v>
+      </c>
+      <c r="V10" s="7">
+        <v>1718952854.7392199</v>
+      </c>
+      <c r="W10" s="7">
+        <v>-37671032.541643202</v>
+      </c>
+      <c r="X10" s="7">
+        <v>-48702880.547294699</v>
+      </c>
+      <c r="Y10" s="7">
+        <v>-34832577.169397101</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>352140630.55937803</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B11" s="6">
         <v>0.08</v>
       </c>
-      <c r="C7">
-        <v>2441.7245797958599</v>
-      </c>
-      <c r="D7" s="7">
-        <v>13.2898157053168</v>
-      </c>
-      <c r="E7" s="7">
-        <v>-8.0650904447436993</v>
-      </c>
-      <c r="F7" s="7">
-        <v>20.382910900777102</v>
-      </c>
-      <c r="G7" s="7">
-        <v>2543.4392873532202</v>
-      </c>
-      <c r="H7" s="7">
-        <v>-71.354243033971997</v>
-      </c>
-      <c r="I7" s="7">
-        <v>-9.6671530760184101</v>
-      </c>
-      <c r="J7" s="7">
-        <v>-73.814088301716495</v>
-      </c>
-      <c r="K7" s="7">
-        <v>485.13108096400998</v>
+      <c r="C11">
+        <v>1662690100.2637801</v>
+      </c>
+      <c r="D11" s="7">
+        <v>44631028.642312303</v>
+      </c>
+      <c r="E11" s="7">
+        <v>-53870825.145849697</v>
+      </c>
+      <c r="F11" s="7">
+        <v>42858109.674520902</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1697874710.61129</v>
+      </c>
+      <c r="H11" s="7">
+        <v>-40229262.9549798</v>
+      </c>
+      <c r="I11" s="7">
+        <v>-50986752.507453904</v>
+      </c>
+      <c r="J11" s="7">
+        <v>-37311702.137431502</v>
+      </c>
+      <c r="K11" s="7">
+        <v>341944057.71948701</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="R11">
+        <v>1662690100.2637801</v>
+      </c>
+      <c r="S11" s="7">
+        <v>44631028.642312303</v>
+      </c>
+      <c r="T11" s="7">
+        <v>-53870825.145849697</v>
+      </c>
+      <c r="U11" s="7">
+        <v>42858109.674520902</v>
+      </c>
+      <c r="V11" s="7">
+        <v>1697874710.61129</v>
+      </c>
+      <c r="W11" s="7">
+        <v>-40229262.9549798</v>
+      </c>
+      <c r="X11" s="7">
+        <v>-50986752.507453904</v>
+      </c>
+      <c r="Y11" s="7">
+        <v>-37311702.137431502</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>341944057.71948701</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="C8">
-        <v>3837.21792541782</v>
-      </c>
-      <c r="D8" s="7">
-        <v>207.80580231433899</v>
-      </c>
-      <c r="E8" s="7">
-        <v>221.231677677785</v>
-      </c>
-      <c r="F8" s="7">
-        <v>210.04935590016399</v>
-      </c>
-      <c r="G8" s="7">
-        <v>3734.22542610454</v>
-      </c>
-      <c r="H8" s="7">
-        <v>421.54242079011499</v>
-      </c>
-      <c r="I8" s="7">
-        <v>220.69408854762801</v>
-      </c>
-      <c r="J8" s="7">
-        <v>420.42892621605802</v>
-      </c>
-      <c r="K8" s="7">
-        <v>1050.40903293614</v>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="C12">
+        <v>1647430283.5880899</v>
+      </c>
+      <c r="D12" s="7">
+        <v>43353041.206873402</v>
+      </c>
+      <c r="E12" s="7">
+        <v>-55875547.492941201</v>
+      </c>
+      <c r="F12" s="7">
+        <v>41542787.465746596</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1680541205.4347301</v>
+      </c>
+      <c r="H12" s="7">
+        <v>-42405800.102588303</v>
+      </c>
+      <c r="I12" s="7">
+        <v>-52929554.844482496</v>
+      </c>
+      <c r="J12" s="7">
+        <v>-39385145.744099602</v>
+      </c>
+      <c r="K12" s="7">
+        <v>333520386.40840602</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="R12">
+        <v>1647430283.5880899</v>
+      </c>
+      <c r="S12" s="7">
+        <v>43353041.206873402</v>
+      </c>
+      <c r="T12" s="7">
+        <v>-55875547.492941201</v>
+      </c>
+      <c r="U12" s="7">
+        <v>41542787.465746596</v>
+      </c>
+      <c r="V12" s="7">
+        <v>1680541205.4347301</v>
+      </c>
+      <c r="W12" s="7">
+        <v>-42405800.102588303</v>
+      </c>
+      <c r="X12" s="7">
+        <v>-52929554.844482496</v>
+      </c>
+      <c r="Y12" s="7">
+        <v>-39385145.744099602</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>333520386.40840602</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="6">
-        <v>0.32</v>
-      </c>
-      <c r="C9">
-        <v>1651.16549676006</v>
-      </c>
-      <c r="D9" s="7">
-        <v>11.747819730912999</v>
-      </c>
-      <c r="E9" s="7">
-        <v>28.472437942975901</v>
-      </c>
-      <c r="F9" s="7">
-        <v>10.1671353251332</v>
-      </c>
-      <c r="G9" s="7">
-        <v>2358.5053043222001</v>
-      </c>
-      <c r="H9" s="7">
-        <v>128.87018324131401</v>
-      </c>
-      <c r="I9" s="7">
-        <v>27.742876947719601</v>
-      </c>
-      <c r="J9" s="7">
-        <v>131.01183412173299</v>
-      </c>
-      <c r="K9" s="7">
-        <v>209.49603349467299</v>
+    <row r="13" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C13">
+        <v>1634629202.83779</v>
+      </c>
+      <c r="D13" s="7">
+        <v>42283229.505063698</v>
+      </c>
+      <c r="E13" s="7">
+        <v>-57599044.825210698</v>
+      </c>
+      <c r="F13" s="7">
+        <v>40440854.412757099</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1665944400.1963601</v>
+      </c>
+      <c r="H13" s="7">
+        <v>-44290987.609665699</v>
+      </c>
+      <c r="I13" s="7">
+        <v>-54619959.289673798</v>
+      </c>
+      <c r="J13" s="7">
+        <v>-41151499.8668897</v>
+      </c>
+      <c r="K13" s="7">
+        <v>326377888.19770199</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="R13">
+        <v>1634629202.83779</v>
+      </c>
+      <c r="S13" s="7">
+        <v>42283229.505063698</v>
+      </c>
+      <c r="T13" s="7">
+        <v>-57599044.825210698</v>
+      </c>
+      <c r="U13" s="7">
+        <v>40440854.412757099</v>
+      </c>
+      <c r="V13" s="7">
+        <v>1665944400.1963601</v>
+      </c>
+      <c r="W13" s="7">
+        <v>-44290987.609665699</v>
+      </c>
+      <c r="X13" s="7">
+        <v>-54619959.289673798</v>
+      </c>
+      <c r="Y13" s="7">
+        <v>-41151499.8668897</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>326377888.19770199</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="3">
-        <v>0.64</v>
-      </c>
-      <c r="C10">
-        <v>1774.9440727178701</v>
-      </c>
-      <c r="D10" s="7">
-        <v>6.5111155206910096</v>
-      </c>
-      <c r="E10" s="7">
-        <v>57.113392909110303</v>
-      </c>
-      <c r="F10" s="7">
-        <v>4.9157215855259704</v>
-      </c>
-      <c r="G10" s="7">
-        <v>2006.0377739957501</v>
-      </c>
-      <c r="H10" s="7">
-        <v>42.754518218258703</v>
-      </c>
-      <c r="I10" s="7">
-        <v>64.272528087686794</v>
-      </c>
-      <c r="J10" s="7">
-        <v>37.703050505763301</v>
-      </c>
-      <c r="K10" s="7">
-        <v>240.549107507809</v>
+    <row r="14" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="9">
+        <f>AVERAGEA(C4:C12)</f>
+        <v>1822300104.5150168</v>
+      </c>
+      <c r="D14" s="10">
+        <f>AVERAGEA(D4:D12)</f>
+        <v>57539584.929976307</v>
+      </c>
+      <c r="E14" s="10">
+        <f>AVERAGEA(E4:E12)</f>
+        <v>-35998477.723082252</v>
+      </c>
+      <c r="F14" s="10">
+        <f>AVERAGEA(F4:F12)</f>
+        <v>56890851.768253356</v>
+      </c>
+      <c r="G14" s="10">
+        <f>AVERAGEA(G4:G12)</f>
+        <v>1869432773.2360954</v>
+      </c>
+      <c r="H14" s="10">
+        <f>AVERAGEA(H4:H12)</f>
+        <v>-22034927.208231732</v>
+      </c>
+      <c r="I14" s="10">
+        <f>AVERAGEA(I4:I12)</f>
+        <v>-33871966.865319677</v>
+      </c>
+      <c r="J14" s="10">
+        <f>AVERAGEA(J4:J12)</f>
+        <v>-21180091.230751906</v>
+      </c>
+      <c r="K14" s="10">
+        <f>AVERAGEA(K4:K12)</f>
+        <v>427509933.34678978</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R14" s="9">
+        <f>AVERAGEA(R4:R12)</f>
+        <v>1822900185.4385545</v>
+      </c>
+      <c r="S14" s="10">
+        <f>AVERAGEA(S4:S12)</f>
+        <v>58507464.55768691</v>
+      </c>
+      <c r="T14" s="10">
+        <f>AVERAGEA(T4:T12)</f>
+        <v>-36314469.444346301</v>
+      </c>
+      <c r="U14" s="10">
+        <f>AVERAGEA(U4:U12)</f>
+        <v>56770237.964463949</v>
+      </c>
+      <c r="V14" s="10">
+        <f>AVERAGEA(V4:V12)</f>
+        <v>1874631840.3005667</v>
+      </c>
+      <c r="W14" s="10">
+        <f>AVERAGEA(W4:W12)</f>
+        <v>-22504683.467400789</v>
+      </c>
+      <c r="X14" s="10">
+        <f>AVERAGEA(X4:X12)</f>
+        <v>-32710213.381823201</v>
+      </c>
+      <c r="Y14" s="10">
+        <f>AVERAGEA(Y4:Y12)</f>
+        <v>-16882247.995843425</v>
+      </c>
+      <c r="Z14" s="10">
+        <f>AVERAGEA(Z4:Z12)</f>
+        <v>427911988.04701263</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="6">
-        <v>0.84</v>
-      </c>
-      <c r="C11">
-        <v>2312.8243541470802</v>
-      </c>
-      <c r="D11" s="7">
-        <v>20.106867917505301</v>
-      </c>
-      <c r="E11" s="7">
-        <v>-110.586619880323</v>
-      </c>
-      <c r="F11" s="7">
-        <v>20.532608087494101</v>
-      </c>
-      <c r="G11" s="7">
-        <v>2278.1066615201098</v>
-      </c>
-      <c r="H11" s="7">
-        <v>-102.794114369748</v>
-      </c>
-      <c r="I11" s="7">
-        <v>-108.501817073186</v>
-      </c>
-      <c r="J11" s="7">
-        <v>-106.3424810918</v>
-      </c>
-      <c r="K11" s="7">
-        <v>351.689425069381</v>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="9">
+        <f>_xlfn.STDEV.P(C4:C12)</f>
+        <v>211575016.02629361</v>
+      </c>
+      <c r="D15" s="10">
+        <f>_xlfn.STDEV.P(D4:D12)</f>
+        <v>17209729.304642465</v>
+      </c>
+      <c r="E15" s="10">
+        <f>_xlfn.STDEV.P(E4:E12)</f>
+        <v>22777216.258799344</v>
+      </c>
+      <c r="F15" s="10">
+        <f>_xlfn.STDEV.P(F4:F12)</f>
+        <v>18572247.320677239</v>
+      </c>
+      <c r="G15" s="10">
+        <f>_xlfn.STDEV.P(G4:G12)</f>
+        <v>224460925.70709828</v>
+      </c>
+      <c r="H15" s="10">
+        <f>_xlfn.STDEV.P(H4:H12)</f>
+        <v>22907636.372779906</v>
+      </c>
+      <c r="I15" s="10">
+        <f>_xlfn.STDEV.P(I4:I12)</f>
+        <v>21857044.629899792</v>
+      </c>
+      <c r="J15" s="10">
+        <f>_xlfn.STDEV.P(J4:J12)</f>
+        <v>18205289.851816628</v>
+      </c>
+      <c r="K15" s="10">
+        <f>_xlfn.STDEV.P(K4:K12)</f>
+        <v>114191242.45205595</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R15" s="9">
+        <f>_xlfn.STDEV.P(R4:R12)</f>
+        <v>213227477.35620502</v>
+      </c>
+      <c r="S15" s="10">
+        <f>_xlfn.STDEV.P(S4:S12)</f>
+        <v>18812980.914154399</v>
+      </c>
+      <c r="T15" s="10">
+        <f>_xlfn.STDEV.P(T4:T12)</f>
+        <v>22280223.760238457</v>
+      </c>
+      <c r="U15" s="10">
+        <f>_xlfn.STDEV.P(U4:U12)</f>
+        <v>18261152.812459774</v>
+      </c>
+      <c r="V15" s="10">
+        <f>_xlfn.STDEV.P(V4:V12)</f>
+        <v>237379072.90440848</v>
+      </c>
+      <c r="W15" s="10">
+        <f>_xlfn.STDEV.P(W4:W12)</f>
+        <v>21816199.837275058</v>
+      </c>
+      <c r="X15" s="10">
+        <f>_xlfn.STDEV.P(X4:X12)</f>
+        <v>24753507.333767734</v>
+      </c>
+      <c r="Y15" s="10">
+        <f>_xlfn.STDEV.P(Y4:Y12)</f>
+        <v>28645615.039940193</v>
+      </c>
+      <c r="Z15" s="10">
+        <f>_xlfn.STDEV.P(Z4:Z12)</f>
+        <v>115198498.25832099</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>2450.7967912035901</v>
-      </c>
-      <c r="D12" s="7">
-        <v>152.31623757459599</v>
-      </c>
-      <c r="E12" s="7">
-        <v>66.649852041400393</v>
-      </c>
-      <c r="F12" s="7">
-        <v>150.052604795143</v>
-      </c>
-      <c r="G12" s="7">
-        <v>2462.97302699281</v>
-      </c>
-      <c r="H12" s="7">
-        <v>-0.85032153708717095</v>
-      </c>
-      <c r="I12" s="7">
-        <v>68.777145392852006</v>
-      </c>
-      <c r="J12" s="7">
-        <v>3.6199618616344999E-2</v>
-      </c>
-      <c r="K12" s="7">
-        <v>680.35616504010295</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="9">
-        <f>AVERAGEA(C4:C12)</f>
-        <v>2582.6451513132179</v>
-      </c>
-      <c r="D13" s="10">
-        <f>AVERAGEA(D4:D12)</f>
-        <v>28.420004137057624</v>
-      </c>
-      <c r="E13" s="10">
-        <f>AVERAGEA(E4:E12)</f>
-        <v>23.169014367346467</v>
-      </c>
-      <c r="F13" s="10">
-        <f>AVERAGEA(F4:F12)</f>
-        <v>70.119689472878648</v>
-      </c>
-      <c r="G13" s="10">
-        <f>AVERAGEA(G4:G12)</f>
-        <v>2621.9129361346836</v>
-      </c>
-      <c r="H13" s="10">
-        <f>AVERAGEA(H4:H12)</f>
-        <v>46.359510634074319</v>
-      </c>
-      <c r="I13" s="10">
-        <f>AVERAGEA(I4:I12)</f>
-        <v>29.227190966284645</v>
-      </c>
-      <c r="J13" s="10">
-        <f>AVERAGEA(J4:J12)</f>
-        <v>31.765332131073492</v>
-      </c>
-      <c r="K13" s="10">
-        <f>AVERAGEA(K4:K12)</f>
-        <v>568.05206447923513</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9">
-        <f>_xlfn.STDEV.P(C4:C12)</f>
-        <v>661.94093343785255</v>
-      </c>
-      <c r="D14" s="10">
-        <f>_xlfn.STDEV.P(D4:D12)</f>
-        <v>123.18323213934735</v>
-      </c>
-      <c r="E14" s="10">
-        <f>_xlfn.STDEV.P(E4:E12)</f>
-        <v>93.448937662997224</v>
-      </c>
-      <c r="F14" s="10">
-        <f>_xlfn.STDEV.P(F4:F12)</f>
-        <v>68.236082893274386</v>
-      </c>
-      <c r="G14" s="10">
-        <f>_xlfn.STDEV.P(G4:G12)</f>
-        <v>530.58682151429809</v>
-      </c>
-      <c r="H14" s="10">
-        <f>_xlfn.STDEV.P(H4:H12)</f>
-        <v>159.27299267321433</v>
-      </c>
-      <c r="I14" s="10">
-        <f>_xlfn.STDEV.P(I4:I12)</f>
-        <v>97.306676766775766</v>
-      </c>
-      <c r="J14" s="10">
-        <f>_xlfn.STDEV.P(J4:J12)</f>
-        <v>155.66832453962346</v>
-      </c>
-      <c r="K14" s="10">
-        <f>_xlfn.STDEV.P(K4:K12)</f>
-        <v>313.5200174267186</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="12" t="s">
+    <row r="16" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="13">
-        <f>C14/C13</f>
-        <v>0.25630347750300508</v>
-      </c>
-      <c r="D15" s="14">
-        <f t="shared" ref="D15:K15" si="0">D14/D13</f>
-        <v>4.33438473637396</v>
-      </c>
-      <c r="E15" s="14">
+      <c r="C16" s="13">
+        <f>C15/C14</f>
+        <v>0.11610327821530897</v>
+      </c>
+      <c r="D16" s="14">
+        <f t="shared" ref="D16:K16" si="0">D15/D14</f>
+        <v>0.29909373391528826</v>
+      </c>
+      <c r="E16" s="14">
         <f t="shared" si="0"/>
-        <v>4.0333583544538101</v>
-      </c>
-      <c r="F15" s="14">
+        <v>-0.63272720680059691</v>
+      </c>
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
-        <v>0.97313726581272419</v>
-      </c>
-      <c r="G15" s="14">
+        <v>0.32645402104949778</v>
+      </c>
+      <c r="G16" s="14">
         <f t="shared" si="0"/>
-        <v>0.20236630065089342</v>
-      </c>
-      <c r="H15" s="15">
+        <v>0.12006900110055498</v>
+      </c>
+      <c r="H16" s="15">
         <f t="shared" si="0"/>
-        <v>3.4356055638807459</v>
-      </c>
-      <c r="I15" s="14">
+        <v>-1.0396057203321347</v>
+      </c>
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
-        <v>3.3293201826691101</v>
-      </c>
-      <c r="J15" s="14">
+        <v>-0.64528418785973884</v>
+      </c>
+      <c r="J16" s="14">
         <f t="shared" si="0"/>
-        <v>4.9005728602895839</v>
-      </c>
-      <c r="K15" s="14">
+        <v>-0.85954728209026365</v>
+      </c>
+      <c r="K16" s="14">
         <f t="shared" si="0"/>
-        <v>0.55192127100909283</v>
+        <v>0.26710781094161312</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" s="13">
+        <f>R15/R14</f>
+        <v>0.11697155941914977</v>
+      </c>
+      <c r="S16" s="14">
+        <f t="shared" ref="S16:Z16" si="1">S15/S14</f>
+        <v>0.32154838799424074</v>
+      </c>
+      <c r="T16" s="14">
+        <f t="shared" si="1"/>
+        <v>-0.61353570907552402</v>
+      </c>
+      <c r="U16" s="14">
+        <f t="shared" si="1"/>
+        <v>0.3216677165223541</v>
+      </c>
+      <c r="V16" s="14">
+        <f t="shared" si="1"/>
+        <v>0.12662703566709324</v>
+      </c>
+      <c r="W16" s="15">
+        <f t="shared" si="1"/>
+        <v>-0.96940709558865668</v>
+      </c>
+      <c r="X16" s="14">
+        <f t="shared" si="1"/>
+        <v>-0.75675163120528766</v>
+      </c>
+      <c r="Y16" s="14">
+        <f t="shared" si="1"/>
+        <v>-1.696789138922318</v>
+      </c>
+      <c r="Z16" s="14">
+        <f t="shared" si="1"/>
+        <v>0.26921072901950266</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:Z2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C15:K15">
+  <conditionalFormatting sqref="C16:K16">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R16:Z16">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corrected indexes of tensor coefficients in graphs
</commit_message>
<xml_diff>
--- a/Results_and_analysis/Dependence_tensor_on_cross_section/results_analysis_complete_cross_section.xlsx
+++ b/Results_and_analysis/Dependence_tensor_on_cross_section/results_analysis_complete_cross_section.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plocha\Bachelor_thesis\Results_and_analysis\Dependence_tensor_on_cross_section\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plocha\Bachelor_thesis\Python_scripts\Results_and_analysis\Dependence_tensor_on_cross_section\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA0D34C-6035-4B01-A477-5CEDE296089C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5132BCF-BE33-4505-8312-62C530AE7E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{434BF738-8343-4BA8-9715-0445CC697F35}"/>
   </bookViews>
@@ -36,33 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>μ</t>
   </si>
   <si>
@@ -79,6 +52,33 @@
   </si>
   <si>
     <t>COEFFICIENTS OF EFFECTIVE ELASTIC TENSOR - COMPRESSION</t>
+  </si>
+  <si>
+    <t>C1111</t>
+  </si>
+  <si>
+    <t>C2211</t>
+  </si>
+  <si>
+    <t>C1211</t>
+  </si>
+  <si>
+    <t>C1112</t>
+  </si>
+  <si>
+    <t>C2222</t>
+  </si>
+  <si>
+    <t>C2212</t>
+  </si>
+  <si>
+    <t>C1122</t>
+  </si>
+  <si>
+    <t>C1222</t>
+  </si>
+  <si>
+    <t>C1212</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -186,15 +186,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -265,12 +256,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,40 +310,50 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -543,7 +581,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>C1</c:v>
+            <c:v>C1111</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -658,7 +696,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>C2</c:v>
+            <c:v>C2211</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -773,7 +811,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>C3</c:v>
+            <c:strRef>
+              <c:f>List1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1211</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -888,7 +934,15 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>C4</c:v>
+            <c:strRef>
+              <c:f>List1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1122</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1003,7 +1057,15 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>C5</c:v>
+            <c:strRef>
+              <c:f>List1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C2222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1118,7 +1180,15 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>C6</c:v>
+            <c:strRef>
+              <c:f>List1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1233,7 +1303,15 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>C7</c:v>
+            <c:strRef>
+              <c:f>List1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1112</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1354,7 +1432,15 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>C8</c:v>
+            <c:strRef>
+              <c:f>List1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C2212</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1475,7 +1561,15 @@
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>C9</c:v>
+            <c:strRef>
+              <c:f>List1!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1212</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1777,8 +1871,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ"/>
-                  <a:t>Hodnota efektivních konstant</a:t>
+                  <a:rPr lang="cs-CZ" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Hodnota efektivních konstant [Pa]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2032,7 +2133,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>C1</c:v>
+            <c:strRef>
+              <c:f>List1!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1111</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2147,7 +2256,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>C2</c:v>
+            <c:strRef>
+              <c:f>List1!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C2211</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2262,7 +2379,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>C3</c:v>
+            <c:strRef>
+              <c:f>List1!$T$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1211</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2377,7 +2502,15 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>C4</c:v>
+            <c:strRef>
+              <c:f>List1!$U$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1122</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2492,7 +2625,15 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>C5</c:v>
+            <c:strRef>
+              <c:f>List1!$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C2222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2607,7 +2748,15 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>C6</c:v>
+            <c:strRef>
+              <c:f>List1!$W$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2722,7 +2871,15 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>C7</c:v>
+            <c:strRef>
+              <c:f>List1!$X$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1112</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2843,7 +3000,15 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>C8</c:v>
+            <c:strRef>
+              <c:f>List1!$Y$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C2212</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2964,7 +3129,15 @@
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>C9</c:v>
+            <c:strRef>
+              <c:f>List1!$Z$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1212</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3267,11 +3440,19 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Hodnota efektivních konstant</a:t>
+                  <a:t>Hodnota efektivních konstant [Pa]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3106508817600702E-2"/>
+              <c:y val="0.33502523896020725"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4914,12 +5095,12 @@
   <dimension ref="B1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+      <selection activeCell="S57" sqref="S57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28.54296875" bestFit="1" customWidth="1"/>
     <col min="18" max="26" width="15.453125" bestFit="1" customWidth="1"/>
@@ -4927,91 +5108,91 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17" t="s">
-        <v>12</v>
+      <c r="B2" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="Q2" s="17" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="17"/>
+      <c r="Q2" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="17"/>
     </row>
     <row r="3" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="18"/>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
+      <c r="B3" s="15"/>
+      <c r="C3" s="18" t="s">
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="U3" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.35">
@@ -5021,28 +5202,28 @@
       <c r="C4" s="4">
         <v>2348434433.5337701</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>100451065.527909</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>19845860.245272499</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>102933897.496317</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>2425339833.0624099</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>33809222.398981698</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>19585310.3809288</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>18533668.903669499</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="20">
         <v>713243397.28215098</v>
       </c>
       <c r="Q4" s="3">
@@ -5051,90 +5232,90 @@
       <c r="R4" s="4">
         <v>2354465672.4657001</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="4">
         <v>105740501.36530399</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="4">
         <v>18247660.305660401</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="4">
         <v>101795217.65406799</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="4">
         <v>2471800046.8102102</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="4">
         <v>29824250.833563101</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="4">
         <v>30041091.732397102</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="4">
         <v>57214258.017845802</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="20">
         <v>716861889.58415699</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.02</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>1985055457.4479699</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>70821950.867204696</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>-17796521.9256359</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>71443231.415179506</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>2043896598.05389</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>-3324531.1763485</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>-15996358.8687004</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>-538615.47619490698</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="21">
         <v>512068013.39598799</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>0.02</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="6">
         <v>1984837287.03004</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="6">
         <v>72488992.228721395</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="6">
         <v>-18465232.9993321</v>
       </c>
-      <c r="U5" s="7">
+      <c r="U5" s="6">
         <v>71454520.490679905</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="6">
         <v>2044259773.5499499</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="6">
         <v>-3535934.06757739</v>
       </c>
-      <c r="X5" s="7">
+      <c r="X5" s="6">
         <v>-15996358.8687004</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Y5" s="6">
         <v>-538615.47619490698</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="Z5" s="21">
         <v>512068013.39598799</v>
       </c>
     </row>
@@ -5142,123 +5323,123 @@
       <c r="B6" s="3">
         <v>0.03</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>1852427823.27141</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>59564568.213844299</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>-31849198.054356199</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>59666946.698082097</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>1904063940.8522201</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>-17689999.295574401</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>-29983955.871647801</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>-14735444.4272255</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="21">
         <v>442579153.78078401</v>
       </c>
       <c r="Q6" s="3">
         <v>0.03</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="6">
         <v>1852215801.2544899</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="6">
         <v>60594575.650751904</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="6">
         <v>-32208001.899628699</v>
       </c>
-      <c r="U6" s="7">
+      <c r="U6" s="6">
         <v>59708813.230726004</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="6">
         <v>1904032155.1886001</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="6">
         <v>-17721431.171448398</v>
       </c>
-      <c r="X6" s="7">
+      <c r="X6" s="6">
         <v>-29983955.871647801</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Y6" s="6">
         <v>-14735444.4272255</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="Z6" s="21">
         <v>442579153.78078401</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.04</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>1781637161.21468</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>53969184.625737898</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>-39630076.294682197</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>53284885.443142898</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>1828700037.06126</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>-25508569.3399878</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>-37516436.928591803</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>-22648176.148858499</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="21">
         <v>405438349.42229903</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>0.04</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="6">
         <v>1781497863.3529</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="6">
         <v>54516327.467568897</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="6">
         <v>-39806112.892950602</v>
       </c>
-      <c r="U7" s="7">
+      <c r="U7" s="6">
         <v>53284885.443142898</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="6">
         <v>1828700037.06126</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="6">
         <v>-25508569.3399878</v>
       </c>
-      <c r="X7" s="7">
+      <c r="X7" s="6">
         <v>-37516436.928591803</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Y7" s="6">
         <v>-22648176.148858499</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z7" s="21">
         <v>405438349.42229903</v>
       </c>
     </row>
@@ -5266,123 +5447,123 @@
       <c r="B8" s="3">
         <v>0.05</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>1736618346.0926399</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>50656621.985981204</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>-44775736.351110399</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>49288956.961299904</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>1780116252.25035</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>-30709209.112047099</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>-42388453.401578203</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>-27911794.4661965</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="21">
         <v>381733886.893727</v>
       </c>
       <c r="Q8" s="3">
         <v>0.05</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="6">
         <v>1736557325.7691801</v>
       </c>
-      <c r="S8" s="7">
+      <c r="S8" s="6">
         <v>50833911.157726496</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="6">
         <v>-44817910.385637604</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8" s="6">
         <v>49288956.961299904</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="6">
         <v>1780116252.25035</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="6">
         <v>-30709209.112047099</v>
       </c>
-      <c r="X8" s="7">
+      <c r="X8" s="6">
         <v>-42388453.401578203</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Y8" s="6">
         <v>-27911794.4661965</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="Z8" s="21">
         <v>381733886.893727</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.06</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>1705038862.71381</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>48207462.722703502</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>-48550179.099549703</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>46527263.374106199</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>1745409527.05949</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>-34585162.749898203</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>-45928619.199056603</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>-31791034.411033001</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="21">
         <v>364921524.65888798</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>0.06</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="6">
         <v>1705038862.71381</v>
       </c>
-      <c r="S9" s="7">
+      <c r="S9" s="6">
         <v>48207462.722703502</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="6">
         <v>-48550179.099549703</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9" s="6">
         <v>46527263.374106199</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="6">
         <v>1745409527.05949</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="6">
         <v>-34585162.749898203</v>
       </c>
-      <c r="X9" s="7">
+      <c r="X9" s="6">
         <v>-45928619.199056603</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Y9" s="6">
         <v>-31791034.411033001</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="21">
         <v>364921524.65888798</v>
       </c>
     </row>
@@ -5390,123 +5571,123 @@
       <c r="B10" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>1681368472.5090001</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>46201340.577220403</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>-51484075.388887502</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>44471587.385885097</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>1718952854.7392199</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>-37671032.541643202</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>-48702880.547294699</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <v>-34832577.169397101</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="21">
         <v>352140630.55937803</v>
       </c>
       <c r="Q10" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="6">
         <v>1681368472.5090001</v>
       </c>
-      <c r="S10" s="7">
+      <c r="S10" s="6">
         <v>46201340.577220403</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="6">
         <v>-51484075.388887502</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10" s="6">
         <v>44471587.385885097</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="6">
         <v>1718952854.7392199</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="6">
         <v>-37671032.541643202</v>
       </c>
-      <c r="X10" s="7">
+      <c r="X10" s="6">
         <v>-48702880.547294699</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Y10" s="6">
         <v>-34832577.169397101</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="Z10" s="21">
         <v>352140630.55937803</v>
       </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.08</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>1662690100.2637801</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>44631028.642312303</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>-53870825.145849697</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>42858109.674520902</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>1697874710.61129</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>-40229262.9549798</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>-50986752.507453904</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>-37311702.137431502</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="21">
         <v>341944057.71948701</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <v>0.08</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="6">
         <v>1662690100.2637801</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="6">
         <v>44631028.642312303</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="6">
         <v>-53870825.145849697</v>
       </c>
-      <c r="U11" s="7">
+      <c r="U11" s="6">
         <v>42858109.674520902</v>
       </c>
-      <c r="V11" s="7">
+      <c r="V11" s="6">
         <v>1697874710.61129</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W11" s="6">
         <v>-40229262.9549798</v>
       </c>
-      <c r="X11" s="7">
+      <c r="X11" s="6">
         <v>-50986752.507453904</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Y11" s="6">
         <v>-37311702.137431502</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11" s="21">
         <v>341944057.71948701</v>
       </c>
     </row>
@@ -5514,61 +5695,61 @@
       <c r="B12" s="3">
         <v>0.09</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>1647430283.5880899</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>43353041.206873402</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>-55875547.492941201</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>41542787.465746596</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>1680541205.4347301</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>-42405800.102588303</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>-52929554.844482496</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>-39385145.744099602</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="21">
         <v>333520386.40840602</v>
       </c>
       <c r="Q12" s="3">
         <v>0.09</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="6">
         <v>1647430283.5880899</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="6">
         <v>43353041.206873402</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <v>-55875547.492941201</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="6">
         <v>41542787.465746596</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="6">
         <v>1680541205.4347301</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="6">
         <v>-42405800.102588303</v>
       </c>
-      <c r="X12" s="7">
+      <c r="X12" s="6">
         <v>-52929554.844482496</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Y12" s="6">
         <v>-39385145.744099602</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="Z12" s="21">
         <v>333520386.40840602</v>
       </c>
     </row>
@@ -5576,301 +5757,301 @@
       <c r="B13" s="3">
         <v>0.1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>1634629202.83779</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>42283229.505063698</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>-57599044.825210698</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>40440854.412757099</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>1665944400.1963601</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>-44290987.609665699</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>-54619959.289673798</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>-41151499.8668897</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="21">
         <v>326377888.19770199</v>
       </c>
       <c r="Q13" s="3">
         <v>0.1</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="6">
         <v>1634629202.83779</v>
       </c>
-      <c r="S13" s="7">
+      <c r="S13" s="6">
         <v>42283229.505063698</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="6">
         <v>-57599044.825210698</v>
       </c>
-      <c r="U13" s="7">
+      <c r="U13" s="6">
         <v>40440854.412757099</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="6">
         <v>1665944400.1963601</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="6">
         <v>-44290987.609665699</v>
       </c>
-      <c r="X13" s="7">
+      <c r="X13" s="6">
         <v>-54619959.289673798</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Y13" s="6">
         <v>-41151499.8668897</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="Z13" s="21">
         <v>326377888.19770199</v>
       </c>
     </row>
     <row r="14" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="9">
-        <f>AVERAGEA(C4:C12)</f>
+      <c r="B14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <f t="shared" ref="C14:K14" si="0">AVERAGEA(C4:C12)</f>
         <v>1822300104.5150168</v>
       </c>
-      <c r="D14" s="10">
-        <f>AVERAGEA(D4:D12)</f>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
         <v>57539584.929976307</v>
       </c>
-      <c r="E14" s="10">
-        <f>AVERAGEA(E4:E12)</f>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
         <v>-35998477.723082252</v>
       </c>
-      <c r="F14" s="10">
-        <f>AVERAGEA(F4:F12)</f>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
         <v>56890851.768253356</v>
       </c>
-      <c r="G14" s="10">
-        <f>AVERAGEA(G4:G12)</f>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
         <v>1869432773.2360954</v>
       </c>
-      <c r="H14" s="10">
-        <f>AVERAGEA(H4:H12)</f>
+      <c r="H14" s="8">
+        <f t="shared" si="0"/>
         <v>-22034927.208231732</v>
       </c>
-      <c r="I14" s="10">
-        <f>AVERAGEA(I4:I12)</f>
+      <c r="I14" s="8">
+        <f t="shared" si="0"/>
         <v>-33871966.865319677</v>
       </c>
-      <c r="J14" s="10">
-        <f>AVERAGEA(J4:J12)</f>
+      <c r="J14" s="8">
+        <f t="shared" si="0"/>
         <v>-21180091.230751906</v>
       </c>
-      <c r="K14" s="10">
-        <f>AVERAGEA(K4:K12)</f>
+      <c r="K14" s="22">
+        <f t="shared" si="0"/>
         <v>427509933.34678978</v>
       </c>
-      <c r="Q14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="R14" s="9">
-        <f>AVERAGEA(R4:R12)</f>
+      <c r="Q14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="8">
+        <f t="shared" ref="R14:Z14" si="1">AVERAGEA(R4:R12)</f>
         <v>1822900185.4385545</v>
       </c>
-      <c r="S14" s="10">
-        <f>AVERAGEA(S4:S12)</f>
+      <c r="S14" s="8">
+        <f t="shared" si="1"/>
         <v>58507464.55768691</v>
       </c>
-      <c r="T14" s="10">
-        <f>AVERAGEA(T4:T12)</f>
+      <c r="T14" s="8">
+        <f t="shared" si="1"/>
         <v>-36314469.444346301</v>
       </c>
-      <c r="U14" s="10">
-        <f>AVERAGEA(U4:U12)</f>
+      <c r="U14" s="8">
+        <f t="shared" si="1"/>
         <v>56770237.964463949</v>
       </c>
-      <c r="V14" s="10">
-        <f>AVERAGEA(V4:V12)</f>
+      <c r="V14" s="8">
+        <f t="shared" si="1"/>
         <v>1874631840.3005667</v>
       </c>
-      <c r="W14" s="10">
-        <f>AVERAGEA(W4:W12)</f>
+      <c r="W14" s="8">
+        <f t="shared" si="1"/>
         <v>-22504683.467400789</v>
       </c>
-      <c r="X14" s="10">
-        <f>AVERAGEA(X4:X12)</f>
+      <c r="X14" s="8">
+        <f t="shared" si="1"/>
         <v>-32710213.381823201</v>
       </c>
-      <c r="Y14" s="10">
-        <f>AVERAGEA(Y4:Y12)</f>
+      <c r="Y14" s="8">
+        <f t="shared" si="1"/>
         <v>-16882247.995843425</v>
       </c>
-      <c r="Z14" s="10">
-        <f>AVERAGEA(Z4:Z12)</f>
+      <c r="Z14" s="22">
+        <f t="shared" si="1"/>
         <v>427911988.04701263</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="9">
-        <f>_xlfn.STDEV.P(C4:C12)</f>
+      <c r="B15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <f t="shared" ref="C15:K15" si="2">_xlfn.STDEV.P(C4:C12)</f>
         <v>211575016.02629361</v>
       </c>
-      <c r="D15" s="10">
-        <f>_xlfn.STDEV.P(D4:D12)</f>
+      <c r="D15" s="8">
+        <f t="shared" si="2"/>
         <v>17209729.304642465</v>
       </c>
-      <c r="E15" s="10">
-        <f>_xlfn.STDEV.P(E4:E12)</f>
+      <c r="E15" s="8">
+        <f t="shared" si="2"/>
         <v>22777216.258799344</v>
       </c>
-      <c r="F15" s="10">
-        <f>_xlfn.STDEV.P(F4:F12)</f>
+      <c r="F15" s="8">
+        <f t="shared" si="2"/>
         <v>18572247.320677239</v>
       </c>
-      <c r="G15" s="10">
-        <f>_xlfn.STDEV.P(G4:G12)</f>
+      <c r="G15" s="8">
+        <f t="shared" si="2"/>
         <v>224460925.70709828</v>
       </c>
-      <c r="H15" s="10">
-        <f>_xlfn.STDEV.P(H4:H12)</f>
+      <c r="H15" s="8">
+        <f t="shared" si="2"/>
         <v>22907636.372779906</v>
       </c>
-      <c r="I15" s="10">
-        <f>_xlfn.STDEV.P(I4:I12)</f>
+      <c r="I15" s="8">
+        <f t="shared" si="2"/>
         <v>21857044.629899792</v>
       </c>
-      <c r="J15" s="10">
-        <f>_xlfn.STDEV.P(J4:J12)</f>
+      <c r="J15" s="8">
+        <f t="shared" si="2"/>
         <v>18205289.851816628</v>
       </c>
-      <c r="K15" s="10">
-        <f>_xlfn.STDEV.P(K4:K12)</f>
+      <c r="K15" s="22">
+        <f t="shared" si="2"/>
         <v>114191242.45205595</v>
       </c>
-      <c r="Q15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R15" s="9">
-        <f>_xlfn.STDEV.P(R4:R12)</f>
+      <c r="Q15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="8">
+        <f t="shared" ref="R15:Z15" si="3">_xlfn.STDEV.P(R4:R12)</f>
         <v>213227477.35620502</v>
       </c>
-      <c r="S15" s="10">
-        <f>_xlfn.STDEV.P(S4:S12)</f>
+      <c r="S15" s="8">
+        <f t="shared" si="3"/>
         <v>18812980.914154399</v>
       </c>
-      <c r="T15" s="10">
-        <f>_xlfn.STDEV.P(T4:T12)</f>
+      <c r="T15" s="8">
+        <f t="shared" si="3"/>
         <v>22280223.760238457</v>
       </c>
-      <c r="U15" s="10">
-        <f>_xlfn.STDEV.P(U4:U12)</f>
+      <c r="U15" s="8">
+        <f t="shared" si="3"/>
         <v>18261152.812459774</v>
       </c>
-      <c r="V15" s="10">
-        <f>_xlfn.STDEV.P(V4:V12)</f>
+      <c r="V15" s="8">
+        <f t="shared" si="3"/>
         <v>237379072.90440848</v>
       </c>
-      <c r="W15" s="10">
-        <f>_xlfn.STDEV.P(W4:W12)</f>
+      <c r="W15" s="8">
+        <f t="shared" si="3"/>
         <v>21816199.837275058</v>
       </c>
-      <c r="X15" s="10">
-        <f>_xlfn.STDEV.P(X4:X12)</f>
+      <c r="X15" s="8">
+        <f t="shared" si="3"/>
         <v>24753507.333767734</v>
       </c>
-      <c r="Y15" s="10">
-        <f>_xlfn.STDEV.P(Y4:Y12)</f>
+      <c r="Y15" s="8">
+        <f t="shared" si="3"/>
         <v>28645615.039940193</v>
       </c>
-      <c r="Z15" s="10">
-        <f>_xlfn.STDEV.P(Z4:Z12)</f>
+      <c r="Z15" s="22">
+        <f t="shared" si="3"/>
         <v>115198498.25832099</v>
       </c>
     </row>
     <row r="16" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="13">
+      <c r="B16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11">
         <f>C15/C14</f>
         <v>0.11610327821530897</v>
       </c>
-      <c r="D16" s="14">
-        <f t="shared" ref="D16:K16" si="0">D15/D14</f>
+      <c r="D16" s="11">
+        <f t="shared" ref="D16:K16" si="4">D15/D14</f>
         <v>0.29909373391528826</v>
       </c>
-      <c r="E16" s="14">
-        <f t="shared" si="0"/>
+      <c r="E16" s="11">
+        <f t="shared" si="4"/>
         <v>-0.63272720680059691</v>
       </c>
-      <c r="F16" s="14">
-        <f t="shared" si="0"/>
+      <c r="F16" s="11">
+        <f t="shared" si="4"/>
         <v>0.32645402104949778</v>
       </c>
-      <c r="G16" s="14">
-        <f t="shared" si="0"/>
+      <c r="G16" s="11">
+        <f t="shared" si="4"/>
         <v>0.12006900110055498</v>
       </c>
-      <c r="H16" s="15">
-        <f t="shared" si="0"/>
+      <c r="H16" s="12">
+        <f t="shared" si="4"/>
         <v>-1.0396057203321347</v>
       </c>
-      <c r="I16" s="14">
-        <f t="shared" si="0"/>
+      <c r="I16" s="11">
+        <f t="shared" si="4"/>
         <v>-0.64528418785973884</v>
       </c>
-      <c r="J16" s="14">
-        <f t="shared" si="0"/>
+      <c r="J16" s="11">
+        <f t="shared" si="4"/>
         <v>-0.85954728209026365</v>
       </c>
-      <c r="K16" s="14">
-        <f t="shared" si="0"/>
+      <c r="K16" s="11">
+        <f t="shared" si="4"/>
         <v>0.26710781094161312</v>
       </c>
-      <c r="Q16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R16" s="13">
+      <c r="Q16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="11">
         <f>R15/R14</f>
         <v>0.11697155941914977</v>
       </c>
-      <c r="S16" s="14">
-        <f t="shared" ref="S16:Z16" si="1">S15/S14</f>
+      <c r="S16" s="11">
+        <f t="shared" ref="S16:Z16" si="5">S15/S14</f>
         <v>0.32154838799424074</v>
       </c>
-      <c r="T16" s="14">
-        <f t="shared" si="1"/>
+      <c r="T16" s="11">
+        <f t="shared" si="5"/>
         <v>-0.61353570907552402</v>
       </c>
-      <c r="U16" s="14">
-        <f t="shared" si="1"/>
+      <c r="U16" s="11">
+        <f t="shared" si="5"/>
         <v>0.3216677165223541</v>
       </c>
-      <c r="V16" s="14">
-        <f t="shared" si="1"/>
+      <c r="V16" s="11">
+        <f t="shared" si="5"/>
         <v>0.12662703566709324</v>
       </c>
-      <c r="W16" s="15">
-        <f t="shared" si="1"/>
+      <c r="W16" s="12">
+        <f t="shared" si="5"/>
         <v>-0.96940709558865668</v>
       </c>
-      <c r="X16" s="14">
-        <f t="shared" si="1"/>
+      <c r="X16" s="11">
+        <f t="shared" si="5"/>
         <v>-0.75675163120528766</v>
       </c>
-      <c r="Y16" s="14">
-        <f t="shared" si="1"/>
+      <c r="Y16" s="11">
+        <f t="shared" si="5"/>
         <v>-1.696789138922318</v>
       </c>
-      <c r="Z16" s="14">
-        <f t="shared" si="1"/>
+      <c r="Z16" s="11">
+        <f t="shared" si="5"/>
         <v>0.26921072901950266</v>
       </c>
     </row>

</xml_diff>